<commit_message>
Deploying to gh-pages from @ mushroomhater07/23_gb_obsinote@19d8ed357d332626e779f519a59c5f05247c80d6 🚀
</commit_message>
<xml_diff>
--- a/01_learning/hehe synology note.xlsx
+++ b/01_learning/hehe synology note.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newhallschool-my.sharepoint.com/personal/chinghey_lau_newhallstudent_co_uk/Documents/00_all/01_Learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newhallschool-my.sharepoint.com/personal/chinghey_lau_newhallstudent_co_uk/Documents/00_all/git/notes/01_learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{458223F6-DA81-4EB4-AD13-CAE654F85969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BF88C20-027E-47F4-97F8-F05B7A8F4E68}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{458223F6-DA81-4EB4-AD13-CAE654F85969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4CD3821-B93C-4CF6-844D-B738C9CA8C38}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3BA4D46D-19F9-4791-86B0-316EFA815065}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22440" windowHeight="13176" xr2:uid="{3BA4D46D-19F9-4791-86B0-316EFA815065}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -902,10 +902,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1207,14 +1203,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB45DA1-BAE9-4AB6-8ED6-F86DC4F17A0A}">
   <dimension ref="A1:G213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" customWidth="1"/>
+    <col min="2" max="2" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1395,66 +1391,64 @@
       <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="D29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="D30" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18.75">
+    <row r="32" spans="1:5" ht="18">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D32" t="s">
-        <v>39</v>
+      <c r="C32" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>40</v>
       </c>
-      <c r="D33" t="s">
-        <v>41</v>
+      <c r="C33" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>42</v>
       </c>
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>43</v>
       </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>44</v>
       </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>45</v>
       </c>
-      <c r="G37" t="s">
-        <v>46</v>
+      <c r="C37" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>47</v>
       </c>
-      <c r="G38" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
@@ -1471,7 +1465,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="18.75">
+    <row r="43" spans="1:7" ht="18">
       <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
@@ -1481,7 +1475,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="18.75">
+    <row r="45" spans="1:7" ht="18">
       <c r="A45" s="1" t="s">
         <v>54</v>
       </c>
@@ -1489,7 +1483,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="18.75">
+    <row r="46" spans="1:7" ht="18">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -1497,7 +1491,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="18.75">
+    <row r="47" spans="1:7" ht="18">
       <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
@@ -1508,7 +1502,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="18.75">
+    <row r="48" spans="1:7" ht="18">
       <c r="A48" s="2" t="s">
         <v>61</v>
       </c>
@@ -1519,7 +1513,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="18.75">
+    <row r="49" spans="1:7" ht="18">
       <c r="A49" s="2" t="s">
         <v>64</v>
       </c>
@@ -1530,7 +1524,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="18.75">
+    <row r="50" spans="1:7" ht="18">
       <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
@@ -1541,7 +1535,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="18.75">
+    <row r="51" spans="1:7" ht="18">
       <c r="A51" s="2" t="s">
         <v>70</v>
       </c>
@@ -1552,7 +1546,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="18.75">
+    <row r="52" spans="1:7" ht="18">
       <c r="A52" t="s">
         <v>73</v>
       </c>
@@ -1563,7 +1557,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="18.75">
+    <row r="53" spans="1:7" ht="18">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -1574,7 +1568,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="18.75">
+    <row r="54" spans="1:7" ht="18">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -1585,7 +1579,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="18.75">
+    <row r="55" spans="1:7" ht="18">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -1593,12 +1587,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18.75">
+    <row r="56" spans="1:7" ht="18">
       <c r="G56" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18.75">
+    <row r="57" spans="1:7" ht="18">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -1606,7 +1600,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="18.75">
+    <row r="58" spans="1:7" ht="18">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -1614,7 +1608,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="18.75">
+    <row r="59" spans="1:7" ht="18">
       <c r="A59" t="s">
         <v>89</v>
       </c>
@@ -1622,7 +1616,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="18.75">
+    <row r="60" spans="1:7" ht="18">
       <c r="A60" t="s">
         <v>91</v>
       </c>
@@ -2026,168 +2020,184 @@
         <v>182</v>
       </c>
     </row>
-    <row r="118" spans="2:3">
-      <c r="B118" t="s">
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="119" spans="2:3">
-      <c r="B119" t="s">
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="120" spans="2:3">
-      <c r="B120" t="s">
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="121" spans="2:3">
-      <c r="B121" t="s">
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="122" spans="2:3">
-      <c r="B122" t="s">
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="123" spans="2:3">
-      <c r="B123" t="s">
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="124" spans="2:3">
-      <c r="B124" t="s">
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="125" spans="2:3">
-      <c r="B125" t="s">
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="126" spans="2:3">
-      <c r="B126" t="s">
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="127" spans="2:3">
-      <c r="B127" t="s">
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>194</v>
       </c>
       <c r="C127" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>197</v>
+      </c>
       <c r="B129" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="B130" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
         <v>196</v>
       </c>
-      <c r="B131" t="s">
-        <v>197</v>
-      </c>
-      <c r="C131" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
+    </row>
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
         <v>200</v>
       </c>
-      <c r="B134" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3">
+    </row>
+    <row r="135" spans="1:2">
       <c r="A135" t="s">
         <v>202</v>
       </c>
-      <c r="B135" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
+    </row>
+    <row r="136" spans="1:2">
       <c r="A136" t="s">
         <v>204</v>
       </c>
-      <c r="B136" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
+    </row>
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
         <v>206</v>
       </c>
-      <c r="B137" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
+    </row>
+    <row r="138" spans="1:2">
       <c r="A138" t="s">
         <v>208</v>
       </c>
-      <c r="B138" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+    </row>
+    <row r="139" spans="1:2">
       <c r="A139" t="s">
         <v>210</v>
       </c>
-      <c r="B139" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
+    </row>
+    <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>212</v>
       </c>
-      <c r="B140" t="s">
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
-      <c r="B141" t="s">
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
-      <c r="B142" t="s">
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
-      <c r="B143" t="s">
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
-      <c r="B144" t="s">
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="145" spans="2:2">
-      <c r="B145" t="s">
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
         <v>218</v>
       </c>
     </row>

</xml_diff>